<commit_message>
Correcting ABP change of rate formula
</commit_message>
<xml_diff>
--- a/Data_Clean/Crime_Rates_1990_2023.xlsx
+++ b/Data_Clean/Crime_Rates_1990_2023.xlsx
@@ -380,10 +380,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1990</t>
-        </is>
+      <c r="A2">
+        <v>1990</v>
       </c>
       <c r="B2">
         <v>729.6</v>
@@ -396,10 +394,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>1991</t>
-        </is>
+      <c r="A3">
+        <v>1991</v>
       </c>
       <c r="B3">
         <v>758.2</v>
@@ -412,10 +408,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>1992</t>
-        </is>
+      <c r="A4">
+        <v>1992</v>
       </c>
       <c r="B4">
         <v>757.7</v>
@@ -428,10 +422,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>1993</t>
-        </is>
+      <c r="A5">
+        <v>1993</v>
       </c>
       <c r="B5">
         <v>747.1</v>
@@ -444,10 +436,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>1994</t>
-        </is>
+      <c r="A6">
+        <v>1994</v>
       </c>
       <c r="B6">
         <v>713.6</v>
@@ -460,10 +450,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>1995</t>
-        </is>
+      <c r="A7">
+        <v>1995</v>
       </c>
       <c r="B7">
         <v>684.5</v>
@@ -476,10 +464,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>1996</t>
-        </is>
+      <c r="A8">
+        <v>1996</v>
       </c>
       <c r="B8">
         <v>636.6</v>
@@ -492,10 +478,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>1997</t>
-        </is>
+      <c r="A9">
+        <v>1997</v>
       </c>
       <c r="B9">
         <v>611</v>
@@ -508,10 +492,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>1998</t>
-        </is>
+      <c r="A10">
+        <v>1998</v>
       </c>
       <c r="B10">
         <v>567.6</v>
@@ -524,10 +506,8 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>1999</t>
-        </is>
+      <c r="A11">
+        <v>1999</v>
       </c>
       <c r="B11">
         <v>523</v>
@@ -540,10 +520,8 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2000</t>
-        </is>
+      <c r="A12">
+        <v>2000</v>
       </c>
       <c r="B12">
         <v>506.5</v>
@@ -556,10 +534,8 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>2001</t>
-        </is>
+      <c r="A13">
+        <v>2001</v>
       </c>
       <c r="B13">
         <v>504.518545947605</v>
@@ -572,10 +548,8 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>2002</t>
-        </is>
+      <c r="A14">
+        <v>2002</v>
       </c>
       <c r="B14">
         <v>494.3770533890423</v>
@@ -588,10 +562,8 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>2003</t>
-        </is>
+      <c r="A15">
+        <v>2003</v>
       </c>
       <c r="B15">
         <v>475.8350949315217</v>
@@ -604,10 +576,8 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>2004</t>
-        </is>
+      <c r="A16">
+        <v>2004</v>
       </c>
       <c r="B16">
         <v>486.5379558960883</v>
@@ -620,10 +590,8 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>2005</t>
-        </is>
+      <c r="A17">
+        <v>2005</v>
       </c>
       <c r="B17">
         <v>492.7849968451175</v>
@@ -636,10 +604,8 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>2006</t>
-        </is>
+      <c r="A18">
+        <v>2006</v>
       </c>
       <c r="B18">
         <v>478.729878939534</v>
@@ -652,10 +618,8 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>2007</t>
-        </is>
+      <c r="A19">
+        <v>2007</v>
       </c>
       <c r="B19">
         <v>476.6906984578671</v>
@@ -668,10 +632,8 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>2008</t>
-        </is>
+      <c r="A20">
+        <v>2008</v>
       </c>
       <c r="B20">
         <v>459.8501181300816</v>
@@ -684,10 +646,8 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>2009</t>
-        </is>
+      <c r="A21">
+        <v>2009</v>
       </c>
       <c r="B21">
         <v>434.3288441240097</v>
@@ -700,10 +660,8 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>2010</t>
-        </is>
+      <c r="A22">
+        <v>2010</v>
       </c>
       <c r="B22">
         <v>411.766922442131</v>
@@ -716,10 +674,8 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>2011</t>
-        </is>
+      <c r="A23">
+        <v>2011</v>
       </c>
       <c r="B23">
         <v>389.4013078651203</v>
@@ -732,10 +688,8 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>2012</t>
-        </is>
+      <c r="A24">
+        <v>2012</v>
       </c>
       <c r="B24">
         <v>387.8647797976797</v>
@@ -748,10 +702,8 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>2013</t>
-        </is>
+      <c r="A25">
+        <v>2013</v>
       </c>
       <c r="B25">
         <v>370.3458386471347</v>
@@ -764,10 +716,8 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>2014</t>
-        </is>
+      <c r="A26">
+        <v>2014</v>
       </c>
       <c r="B26">
         <v>363.5607173140305</v>
@@ -780,10 +730,8 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>2015</t>
-        </is>
+      <c r="A27">
+        <v>2015</v>
       </c>
       <c r="B27">
         <v>372.4483214766329</v>
@@ -796,10 +744,8 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>2016</t>
-        </is>
+      <c r="A28">
+        <v>2016</v>
       </c>
       <c r="B28">
         <v>386.8172624471009</v>
@@ -812,10 +758,8 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>2017</t>
-        </is>
+      <c r="A29">
+        <v>2017</v>
       </c>
       <c r="B29">
         <v>376.520353370166</v>
@@ -828,10 +772,8 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>2018</t>
-        </is>
+      <c r="A30">
+        <v>2018</v>
       </c>
       <c r="B30">
         <v>370.8397822993593</v>
@@ -844,10 +786,8 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>2019</t>
-        </is>
+      <c r="A31">
+        <v>2019</v>
       </c>
       <c r="B31">
         <v>364.3639867620383</v>
@@ -860,10 +800,8 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
+      <c r="A32">
+        <v>2020</v>
       </c>
       <c r="B32">
         <v>386.3045018408975</v>
@@ -876,10 +814,8 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
+      <c r="A33">
+        <v>2021</v>
       </c>
       <c r="B33">
         <v>360.9371432693911</v>
@@ -892,10 +828,8 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
+      <c r="A34">
+        <v>2022</v>
       </c>
       <c r="B34">
         <v>377.0530803224676</v>
@@ -908,10 +842,8 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>2023</t>
-        </is>
+      <c r="A35">
+        <v>2023</v>
       </c>
       <c r="B35">
         <v>363.8139175625498</v>

</xml_diff>

<commit_message>
Final updates w BCJ
</commit_message>
<xml_diff>
--- a/Data_Clean/Crime_Rates_1990_2023.xlsx
+++ b/Data_Clean/Crime_Rates_1990_2023.xlsx
@@ -380,10 +380,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1990</t>
-        </is>
+      <c r="A2">
+        <v>1990</v>
       </c>
       <c r="B2">
         <v>729.6</v>
@@ -396,10 +394,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>1991</t>
-        </is>
+      <c r="A3">
+        <v>1991</v>
       </c>
       <c r="B3">
         <v>758.2</v>
@@ -412,10 +408,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>1992</t>
-        </is>
+      <c r="A4">
+        <v>1992</v>
       </c>
       <c r="B4">
         <v>757.7</v>
@@ -428,10 +422,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>1993</t>
-        </is>
+      <c r="A5">
+        <v>1993</v>
       </c>
       <c r="B5">
         <v>747.1</v>
@@ -444,10 +436,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>1994</t>
-        </is>
+      <c r="A6">
+        <v>1994</v>
       </c>
       <c r="B6">
         <v>713.6</v>
@@ -460,10 +450,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>1995</t>
-        </is>
+      <c r="A7">
+        <v>1995</v>
       </c>
       <c r="B7">
         <v>684.5</v>
@@ -476,10 +464,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>1996</t>
-        </is>
+      <c r="A8">
+        <v>1996</v>
       </c>
       <c r="B8">
         <v>636.6</v>
@@ -492,10 +478,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>1997</t>
-        </is>
+      <c r="A9">
+        <v>1997</v>
       </c>
       <c r="B9">
         <v>611</v>
@@ -508,10 +492,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>1998</t>
-        </is>
+      <c r="A10">
+        <v>1998</v>
       </c>
       <c r="B10">
         <v>567.6</v>
@@ -524,10 +506,8 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>1999</t>
-        </is>
+      <c r="A11">
+        <v>1999</v>
       </c>
       <c r="B11">
         <v>523</v>
@@ -540,10 +520,8 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2000</t>
-        </is>
+      <c r="A12">
+        <v>2000</v>
       </c>
       <c r="B12">
         <v>506.5</v>
@@ -556,10 +534,8 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>2001</t>
-        </is>
+      <c r="A13">
+        <v>2001</v>
       </c>
       <c r="B13">
         <v>504.518545947605</v>
@@ -572,10 +548,8 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>2002</t>
-        </is>
+      <c r="A14">
+        <v>2002</v>
       </c>
       <c r="B14">
         <v>494.3770533890423</v>
@@ -588,10 +562,8 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>2003</t>
-        </is>
+      <c r="A15">
+        <v>2003</v>
       </c>
       <c r="B15">
         <v>475.8350949315217</v>
@@ -604,10 +576,8 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>2004</t>
-        </is>
+      <c r="A16">
+        <v>2004</v>
       </c>
       <c r="B16">
         <v>486.5379558960883</v>
@@ -620,10 +590,8 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>2005</t>
-        </is>
+      <c r="A17">
+        <v>2005</v>
       </c>
       <c r="B17">
         <v>492.7849968451175</v>
@@ -636,10 +604,8 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>2006</t>
-        </is>
+      <c r="A18">
+        <v>2006</v>
       </c>
       <c r="B18">
         <v>478.729878939534</v>
@@ -652,10 +618,8 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>2007</t>
-        </is>
+      <c r="A19">
+        <v>2007</v>
       </c>
       <c r="B19">
         <v>476.6906984578671</v>
@@ -668,10 +632,8 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>2008</t>
-        </is>
+      <c r="A20">
+        <v>2008</v>
       </c>
       <c r="B20">
         <v>459.8501181300816</v>
@@ -684,10 +646,8 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>2009</t>
-        </is>
+      <c r="A21">
+        <v>2009</v>
       </c>
       <c r="B21">
         <v>434.3288441240097</v>
@@ -700,10 +660,8 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>2010</t>
-        </is>
+      <c r="A22">
+        <v>2010</v>
       </c>
       <c r="B22">
         <v>411.766922442131</v>
@@ -716,10 +674,8 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>2011</t>
-        </is>
+      <c r="A23">
+        <v>2011</v>
       </c>
       <c r="B23">
         <v>389.4013078651203</v>
@@ -732,10 +688,8 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>2012</t>
-        </is>
+      <c r="A24">
+        <v>2012</v>
       </c>
       <c r="B24">
         <v>387.8647797976797</v>
@@ -748,10 +702,8 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>2013</t>
-        </is>
+      <c r="A25">
+        <v>2013</v>
       </c>
       <c r="B25">
         <v>370.3458386471347</v>
@@ -764,10 +716,8 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>2014</t>
-        </is>
+      <c r="A26">
+        <v>2014</v>
       </c>
       <c r="B26">
         <v>363.5607173140305</v>
@@ -780,10 +730,8 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>2015</t>
-        </is>
+      <c r="A27">
+        <v>2015</v>
       </c>
       <c r="B27">
         <v>372.4483214766329</v>
@@ -796,10 +744,8 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>2016</t>
-        </is>
+      <c r="A28">
+        <v>2016</v>
       </c>
       <c r="B28">
         <v>386.8172624471009</v>
@@ -812,10 +758,8 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>2017</t>
-        </is>
+      <c r="A29">
+        <v>2017</v>
       </c>
       <c r="B29">
         <v>376.520353370166</v>
@@ -828,10 +772,8 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>2018</t>
-        </is>
+      <c r="A30">
+        <v>2018</v>
       </c>
       <c r="B30">
         <v>370.8397822993593</v>
@@ -844,10 +786,8 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>2019</t>
-        </is>
+      <c r="A31">
+        <v>2019</v>
       </c>
       <c r="B31">
         <v>364.3639867620383</v>
@@ -860,10 +800,8 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
+      <c r="A32">
+        <v>2020</v>
       </c>
       <c r="B32">
         <v>386.3045018408975</v>
@@ -876,10 +814,8 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
+      <c r="A33">
+        <v>2021</v>
       </c>
       <c r="B33">
         <v>360.9371432693911</v>
@@ -892,10 +828,8 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
+      <c r="A34">
+        <v>2022</v>
       </c>
       <c r="B34">
         <v>377.0530803224676</v>
@@ -908,10 +842,8 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>2023</t>
-        </is>
+      <c r="A35">
+        <v>2023</v>
       </c>
       <c r="B35">
         <v>363.8139175625498</v>

</xml_diff>